<commit_message>
2015 all semester data merged
</commit_message>
<xml_diff>
--- a/Cleaned-Data/2015-Passouts/Sem-5_2015_Passout_cleaned.xlsx
+++ b/Cleaned-Data/2015-Passouts/Sem-5_2015_Passout_cleaned.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prashant/Downloads/Student-Placement-Guidance/Cleaned-Data/2015-Passouts/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="24600" windowHeight="12280"/>
   </bookViews>
   <sheets>
     <sheet name="Sem-5_2015_Passout_cleaned" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1057,8 +1070,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1121,6 +1134,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1167,12 +1185,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1199,14 +1217,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1233,6 +1252,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1408,14 +1428,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="A171" sqref="A171"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="4" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:39">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,9 +1593,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:39">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>235201</v>
@@ -1599,9 +1661,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:39">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>235202</v>
@@ -1667,9 +1729,9 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:39">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>235203</v>
@@ -1735,9 +1797,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>235204</v>
@@ -1803,9 +1865,9 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:39">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>235205</v>
@@ -1919,9 +1981,9 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:39">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>235206</v>
@@ -2035,9 +2097,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:39">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>235207</v>
@@ -2151,9 +2213,9 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:39">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>235208</v>
@@ -2219,9 +2281,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:39">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>235209</v>
@@ -2287,9 +2349,9 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:39">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>235210</v>
@@ -2355,9 +2417,9 @@
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:39">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>235211</v>
@@ -2423,9 +2485,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:39">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>235212</v>
@@ -2491,9 +2553,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:39">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>235213</v>
@@ -2607,9 +2669,9 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:39">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>235214</v>
@@ -2675,9 +2737,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>235215</v>
@@ -2743,9 +2805,9 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>235216</v>
@@ -2811,9 +2873,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>235217</v>
@@ -2927,9 +2989,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>235218</v>
@@ -2995,9 +3057,9 @@
         <v>238</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>235219</v>
@@ -3063,9 +3125,9 @@
         <v>239</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>235220</v>
@@ -3179,9 +3241,9 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>235221</v>
@@ -3247,9 +3309,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>235222</v>
@@ -3315,9 +3377,9 @@
         <v>237</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>235223</v>
@@ -3383,9 +3445,9 @@
         <v>242</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>235224</v>
@@ -3451,9 +3513,9 @@
         <v>243</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>235225</v>
@@ -3519,9 +3581,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>235226</v>
@@ -3587,9 +3649,9 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>235227</v>
@@ -3703,9 +3765,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>235228</v>
@@ -3819,9 +3881,9 @@
         <v>247</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>235229</v>
@@ -3887,9 +3949,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>235230</v>
@@ -3955,9 +4017,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>235231</v>
@@ -4023,9 +4085,9 @@
         <v>250</v>
       </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>235232</v>
@@ -4091,9 +4153,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>235233</v>
@@ -4159,9 +4221,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>235234</v>
@@ -4227,9 +4289,9 @@
         <v>244</v>
       </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>235235</v>
@@ -4295,9 +4357,9 @@
         <v>253</v>
       </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>235236</v>
@@ -4363,9 +4425,9 @@
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>235237</v>
@@ -4431,9 +4493,9 @@
         <v>245</v>
       </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>235238</v>
@@ -4499,9 +4561,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>235239</v>
@@ -4567,9 +4629,9 @@
         <v>256</v>
       </c>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>235240</v>
@@ -4635,9 +4697,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>235241</v>
@@ -4751,9 +4813,9 @@
         <v>258</v>
       </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>235242</v>
@@ -4819,9 +4881,9 @@
         <v>259</v>
       </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>235243</v>
@@ -4887,9 +4949,9 @@
         <v>260</v>
       </c>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>235244</v>
@@ -4955,9 +5017,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>235245</v>
@@ -5023,9 +5085,9 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>235246</v>
@@ -5139,9 +5201,9 @@
         <v>263</v>
       </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>235247</v>
@@ -5207,9 +5269,9 @@
         <v>264</v>
       </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>235248</v>
@@ -5275,9 +5337,9 @@
         <v>265</v>
       </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>235249</v>
@@ -5391,9 +5453,9 @@
         <v>266</v>
       </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>235250</v>
@@ -5459,9 +5521,9 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>235251</v>
@@ -5575,9 +5637,9 @@
         <v>268</v>
       </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>235252</v>
@@ -5691,9 +5753,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>235253</v>
@@ -5807,9 +5869,9 @@
         <v>270</v>
       </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>235254</v>
@@ -5875,9 +5937,9 @@
         <v>271</v>
       </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>235255</v>
@@ -5943,9 +6005,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>235256</v>
@@ -6011,9 +6073,9 @@
         <v>273</v>
       </c>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>235257</v>
@@ -6079,9 +6141,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:38">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>235258</v>
@@ -6147,9 +6209,9 @@
         <v>274</v>
       </c>
     </row>
-    <row r="60" spans="1:38">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>235259</v>
@@ -6263,9 +6325,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="61" spans="1:38">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>235260</v>
@@ -6331,9 +6393,9 @@
         <v>224</v>
       </c>
     </row>
-    <row r="62" spans="1:38">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>235261</v>
@@ -6399,9 +6461,9 @@
         <v>276</v>
       </c>
     </row>
-    <row r="63" spans="1:38">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>235262</v>
@@ -6467,9 +6529,9 @@
         <v>277</v>
       </c>
     </row>
-    <row r="64" spans="1:38">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>235263</v>
@@ -6583,9 +6645,9 @@
         <v>278</v>
       </c>
     </row>
-    <row r="65" spans="1:38">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>235264</v>
@@ -6651,9 +6713,9 @@
         <v>279</v>
       </c>
     </row>
-    <row r="66" spans="1:38">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>235265</v>
@@ -6719,9 +6781,9 @@
         <v>280</v>
       </c>
     </row>
-    <row r="67" spans="1:38">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>235266</v>
@@ -6835,9 +6897,9 @@
         <v>281</v>
       </c>
     </row>
-    <row r="68" spans="1:38">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>235267</v>
@@ -6951,9 +7013,9 @@
         <v>282</v>
       </c>
     </row>
-    <row r="69" spans="1:38">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>235268</v>
@@ -7019,9 +7081,9 @@
         <v>283</v>
       </c>
     </row>
-    <row r="70" spans="1:38">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>235269</v>
@@ -7087,9 +7149,9 @@
         <v>284</v>
       </c>
     </row>
-    <row r="71" spans="1:38">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B71">
         <v>235270</v>
@@ -7155,9 +7217,9 @@
         <v>285</v>
       </c>
     </row>
-    <row r="72" spans="1:38">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>235271</v>
@@ -7223,9 +7285,9 @@
         <v>286</v>
       </c>
     </row>
-    <row r="73" spans="1:38">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>235272</v>
@@ -7291,9 +7353,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="74" spans="1:38">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>235273</v>
@@ -7407,9 +7469,9 @@
         <v>287</v>
       </c>
     </row>
-    <row r="75" spans="1:38">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>235274</v>
@@ -7475,9 +7537,9 @@
         <v>288</v>
       </c>
     </row>
-    <row r="76" spans="1:38">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B76">
         <v>235275</v>
@@ -7543,9 +7605,9 @@
         <v>264</v>
       </c>
     </row>
-    <row r="77" spans="1:38">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B77">
         <v>235276</v>
@@ -7629,9 +7691,9 @@
         <v>289</v>
       </c>
     </row>
-    <row r="78" spans="1:38">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>235277</v>
@@ -7697,9 +7759,9 @@
         <v>290</v>
       </c>
     </row>
-    <row r="79" spans="1:38">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B79">
         <v>235278</v>
@@ -7765,9 +7827,9 @@
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:38">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>235279</v>
@@ -7833,9 +7895,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="81" spans="1:38">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>235280</v>
@@ -7937,9 +7999,9 @@
         <v>291</v>
       </c>
     </row>
-    <row r="82" spans="1:38">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>235281</v>
@@ -8005,9 +8067,9 @@
         <v>292</v>
       </c>
     </row>
-    <row r="83" spans="1:38">
+    <row r="83" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B83">
         <v>235282</v>
@@ -8121,9 +8183,9 @@
         <v>293</v>
       </c>
     </row>
-    <row r="84" spans="1:38">
+    <row r="84" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B84">
         <v>235283</v>
@@ -8237,9 +8299,9 @@
         <v>294</v>
       </c>
     </row>
-    <row r="85" spans="1:38">
+    <row r="85" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B85">
         <v>235284</v>
@@ -8353,9 +8415,9 @@
         <v>295</v>
       </c>
     </row>
-    <row r="86" spans="1:38">
+    <row r="86" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>235285</v>
@@ -8421,9 +8483,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="87" spans="1:38">
+    <row r="87" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B87">
         <v>235286</v>
@@ -8537,9 +8599,9 @@
         <v>296</v>
       </c>
     </row>
-    <row r="88" spans="1:38">
+    <row r="88" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>235287</v>
@@ -8653,9 +8715,9 @@
         <v>297</v>
       </c>
     </row>
-    <row r="89" spans="1:38">
+    <row r="89" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>235288</v>
@@ -8721,9 +8783,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="90" spans="1:38">
+    <row r="90" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>235289</v>
@@ -8837,9 +8899,9 @@
         <v>281</v>
       </c>
     </row>
-    <row r="91" spans="1:38">
+    <row r="91" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>235290</v>
@@ -8953,9 +9015,9 @@
         <v>298</v>
       </c>
     </row>
-    <row r="92" spans="1:38">
+    <row r="92" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>235291</v>
@@ -9069,9 +9131,9 @@
         <v>299</v>
       </c>
     </row>
-    <row r="93" spans="1:38">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>235292</v>
@@ -9137,9 +9199,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="94" spans="1:38">
+    <row r="94" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>235293</v>
@@ -9253,9 +9315,9 @@
         <v>300</v>
       </c>
     </row>
-    <row r="95" spans="1:38">
+    <row r="95" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>235294</v>
@@ -9369,9 +9431,9 @@
         <v>301</v>
       </c>
     </row>
-    <row r="96" spans="1:38">
+    <row r="96" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>235295</v>
@@ -9485,9 +9547,9 @@
         <v>302</v>
       </c>
     </row>
-    <row r="97" spans="1:38">
+    <row r="97" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>235296</v>
@@ -9553,9 +9615,9 @@
         <v>303</v>
       </c>
     </row>
-    <row r="98" spans="1:38">
+    <row r="98" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>235297</v>
@@ -9621,9 +9683,9 @@
         <v>304</v>
       </c>
     </row>
-    <row r="99" spans="1:38">
+    <row r="99" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>235298</v>
@@ -9737,9 +9799,9 @@
         <v>267</v>
       </c>
     </row>
-    <row r="100" spans="1:38">
+    <row r="100" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>235299</v>
@@ -9805,9 +9867,9 @@
         <v>301</v>
       </c>
     </row>
-    <row r="101" spans="1:38">
+    <row r="101" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>235300</v>
@@ -9873,9 +9935,9 @@
         <v>290</v>
       </c>
     </row>
-    <row r="102" spans="1:38">
+    <row r="102" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>235301</v>
@@ -9941,9 +10003,9 @@
         <v>261</v>
       </c>
     </row>
-    <row r="103" spans="1:38">
+    <row r="103" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>235302</v>
@@ -10009,9 +10071,9 @@
         <v>305</v>
       </c>
     </row>
-    <row r="104" spans="1:38">
+    <row r="104" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>235303</v>
@@ -10077,9 +10139,9 @@
         <v>277</v>
       </c>
     </row>
-    <row r="105" spans="1:38">
+    <row r="105" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>235304</v>
@@ -10145,9 +10207,9 @@
         <v>306</v>
       </c>
     </row>
-    <row r="106" spans="1:38">
+    <row r="106" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>235305</v>
@@ -10261,9 +10323,9 @@
         <v>307</v>
       </c>
     </row>
-    <row r="107" spans="1:38">
+    <row r="107" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B107">
         <v>235306</v>
@@ -10377,9 +10439,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="1:38">
+    <row r="108" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>235307</v>
@@ -10445,9 +10507,9 @@
         <v>308</v>
       </c>
     </row>
-    <row r="109" spans="1:38">
+    <row r="109" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>235308</v>
@@ -10513,9 +10575,9 @@
         <v>309</v>
       </c>
     </row>
-    <row r="110" spans="1:38">
+    <row r="110" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B110">
         <v>235309</v>
@@ -10581,9 +10643,9 @@
         <v>257</v>
       </c>
     </row>
-    <row r="111" spans="1:38">
+    <row r="111" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>235310</v>
@@ -10649,9 +10711,9 @@
         <v>279</v>
       </c>
     </row>
-    <row r="112" spans="1:38">
+    <row r="112" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B112">
         <v>235311</v>
@@ -10717,9 +10779,9 @@
         <v>249</v>
       </c>
     </row>
-    <row r="113" spans="1:38">
+    <row r="113" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B113">
         <v>235312</v>
@@ -10785,9 +10847,9 @@
         <v>290</v>
       </c>
     </row>
-    <row r="114" spans="1:38">
+    <row r="114" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B114">
         <v>235313</v>
@@ -10901,9 +10963,9 @@
         <v>310</v>
       </c>
     </row>
-    <row r="115" spans="1:38">
+    <row r="115" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>235314</v>
@@ -10969,9 +11031,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="116" spans="1:38">
+    <row r="116" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B116">
         <v>235315</v>
@@ -11037,9 +11099,9 @@
         <v>311</v>
       </c>
     </row>
-    <row r="117" spans="1:38">
+    <row r="117" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B117">
         <v>235316</v>
@@ -11105,9 +11167,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="118" spans="1:38">
+    <row r="118" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B118">
         <v>235317</v>
@@ -11173,9 +11235,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="1:38">
+    <row r="119" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B119">
         <v>235318</v>
@@ -11241,9 +11303,9 @@
         <v>313</v>
       </c>
     </row>
-    <row r="120" spans="1:38">
+    <row r="120" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B120">
         <v>235319</v>
@@ -11309,9 +11371,9 @@
         <v>314</v>
       </c>
     </row>
-    <row r="121" spans="1:38">
+    <row r="121" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B121">
         <v>235320</v>
@@ -11377,9 +11439,9 @@
         <v>313</v>
       </c>
     </row>
-    <row r="122" spans="1:38">
+    <row r="122" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B122">
         <v>235321</v>
@@ -11445,9 +11507,9 @@
         <v>315</v>
       </c>
     </row>
-    <row r="123" spans="1:38">
+    <row r="123" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B123">
         <v>235322</v>
@@ -11513,9 +11575,9 @@
         <v>264</v>
       </c>
     </row>
-    <row r="124" spans="1:38">
+    <row r="124" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B124">
         <v>235323</v>
@@ -11629,9 +11691,9 @@
         <v>287</v>
       </c>
     </row>
-    <row r="125" spans="1:38">
+    <row r="125" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B125">
         <v>235324</v>
@@ -11697,9 +11759,9 @@
         <v>248</v>
       </c>
     </row>
-    <row r="126" spans="1:38">
+    <row r="126" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B126">
         <v>235325</v>
@@ -11765,9 +11827,9 @@
         <v>316</v>
       </c>
     </row>
-    <row r="127" spans="1:38">
+    <row r="127" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B127">
         <v>235326</v>
@@ -11833,9 +11895,9 @@
         <v>302</v>
       </c>
     </row>
-    <row r="128" spans="1:38">
+    <row r="128" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B128">
         <v>235327</v>
@@ -11901,9 +11963,9 @@
         <v>317</v>
       </c>
     </row>
-    <row r="129" spans="1:38">
+    <row r="129" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B129">
         <v>235328</v>
@@ -11969,9 +12031,9 @@
         <v>275</v>
       </c>
     </row>
-    <row r="130" spans="1:38">
+    <row r="130" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B130">
         <v>235329</v>
@@ -12037,9 +12099,9 @@
         <v>272</v>
       </c>
     </row>
-    <row r="131" spans="1:38">
+    <row r="131" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>235330</v>
@@ -12153,9 +12215,9 @@
         <v>246</v>
       </c>
     </row>
-    <row r="132" spans="1:38">
+    <row r="132" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>235331</v>
@@ -12221,9 +12283,9 @@
         <v>318</v>
       </c>
     </row>
-    <row r="133" spans="1:38">
+    <row r="133" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B133">
         <v>235332</v>
@@ -12337,9 +12399,9 @@
         <v>301</v>
       </c>
     </row>
-    <row r="134" spans="1:38">
+    <row r="134" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B134">
         <v>235333</v>
@@ -12453,9 +12515,9 @@
         <v>319</v>
       </c>
     </row>
-    <row r="135" spans="1:38">
+    <row r="135" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B135">
         <v>235334</v>
@@ -12569,9 +12631,9 @@
         <v>320</v>
       </c>
     </row>
-    <row r="136" spans="1:38">
+    <row r="136" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B136">
         <v>235335</v>
@@ -12685,9 +12747,9 @@
         <v>280</v>
       </c>
     </row>
-    <row r="137" spans="1:38">
+    <row r="137" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>235336</v>
@@ -12753,9 +12815,9 @@
         <v>277</v>
       </c>
     </row>
-    <row r="138" spans="1:38">
+    <row r="138" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B138">
         <v>235337</v>
@@ -12869,9 +12931,9 @@
         <v>321</v>
       </c>
     </row>
-    <row r="139" spans="1:38">
+    <row r="139" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B139">
         <v>235338</v>
@@ -12937,9 +12999,9 @@
         <v>243</v>
       </c>
     </row>
-    <row r="140" spans="1:38">
+    <row r="140" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B140">
         <v>235339</v>
@@ -13005,9 +13067,9 @@
         <v>322</v>
       </c>
     </row>
-    <row r="141" spans="1:38">
+    <row r="141" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B141">
         <v>235340</v>
@@ -13073,9 +13135,9 @@
         <v>323</v>
       </c>
     </row>
-    <row r="142" spans="1:38">
+    <row r="142" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B142">
         <v>235341</v>
@@ -13189,9 +13251,9 @@
         <v>324</v>
       </c>
     </row>
-    <row r="143" spans="1:38">
+    <row r="143" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B143">
         <v>235342</v>
@@ -13257,9 +13319,9 @@
         <v>325</v>
       </c>
     </row>
-    <row r="144" spans="1:38">
+    <row r="144" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B144">
         <v>235343</v>
@@ -13325,9 +13387,9 @@
         <v>227</v>
       </c>
     </row>
-    <row r="145" spans="1:38">
+    <row r="145" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B145">
         <v>235344</v>
@@ -13441,9 +13503,9 @@
         <v>326</v>
       </c>
     </row>
-    <row r="146" spans="1:38">
+    <row r="146" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B146">
         <v>235345</v>
@@ -13509,9 +13571,9 @@
         <v>277</v>
       </c>
     </row>
-    <row r="147" spans="1:38">
+    <row r="147" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B147">
         <v>235346</v>
@@ -13619,9 +13681,9 @@
         <v>327</v>
       </c>
     </row>
-    <row r="148" spans="1:38">
+    <row r="148" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B148">
         <v>235347</v>
@@ -13735,9 +13797,9 @@
         <v>328</v>
       </c>
     </row>
-    <row r="149" spans="1:38">
+    <row r="149" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B149">
         <v>235348</v>
@@ -13851,9 +13913,9 @@
         <v>329</v>
       </c>
     </row>
-    <row r="150" spans="1:38">
+    <row r="150" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B150">
         <v>235349</v>
@@ -13955,9 +14017,9 @@
         <v>330</v>
       </c>
     </row>
-    <row r="151" spans="1:38">
+    <row r="151" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B151">
         <v>235350</v>
@@ -14059,9 +14121,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="152" spans="1:38">
+    <row r="152" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B152">
         <v>235351</v>
@@ -14175,9 +14237,9 @@
         <v>309</v>
       </c>
     </row>
-    <row r="153" spans="1:38">
+    <row r="153" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B153">
         <v>235352</v>
@@ -14285,9 +14347,9 @@
         <v>332</v>
       </c>
     </row>
-    <row r="154" spans="1:38">
+    <row r="154" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B154">
         <v>235353</v>
@@ -14401,9 +14463,9 @@
         <v>333</v>
       </c>
     </row>
-    <row r="155" spans="1:38">
+    <row r="155" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B155">
         <v>235354</v>
@@ -14508,9 +14570,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="156" spans="1:38">
+    <row r="156" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B156">
         <v>235355</v>
@@ -14606,9 +14668,9 @@
         <v>334</v>
       </c>
     </row>
-    <row r="157" spans="1:38">
+    <row r="157" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B157">
         <v>235356</v>
@@ -14722,9 +14784,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="158" spans="1:38">
+    <row r="158" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B158">
         <v>235357</v>
@@ -14832,9 +14894,9 @@
         <v>335</v>
       </c>
     </row>
-    <row r="159" spans="1:38">
+    <row r="159" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B159">
         <v>235358</v>
@@ -14948,9 +15010,9 @@
         <v>309</v>
       </c>
     </row>
-    <row r="160" spans="1:38">
+    <row r="160" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B160">
         <v>235359</v>
@@ -15061,9 +15123,9 @@
         <v>336</v>
       </c>
     </row>
-    <row r="161" spans="1:38">
+    <row r="161" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B161">
         <v>235360</v>
@@ -15177,9 +15239,9 @@
         <v>337</v>
       </c>
     </row>
-    <row r="162" spans="1:38">
+    <row r="162" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B162" t="s">
         <v>38</v>
@@ -15257,9 +15319,9 @@
         <v>338</v>
       </c>
     </row>
-    <row r="163" spans="1:38">
+    <row r="163" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B163" t="s">
         <v>39</v>
@@ -15349,9 +15411,9 @@
         <v>339</v>
       </c>
     </row>
-    <row r="164" spans="1:38">
+    <row r="164" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B164" t="s">
         <v>40</v>
@@ -15465,9 +15527,9 @@
         <v>340</v>
       </c>
     </row>
-    <row r="165" spans="1:38">
+    <row r="165" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B165" t="s">
         <v>41</v>
@@ -15581,9 +15643,9 @@
         <v>341</v>
       </c>
     </row>
-    <row r="166" spans="1:38">
+    <row r="166" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B166" t="s">
         <v>42</v>
@@ -15697,9 +15759,9 @@
         <v>342</v>
       </c>
     </row>
-    <row r="167" spans="1:38">
+    <row r="167" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B167" t="s">
         <v>43</v>
@@ -15813,9 +15875,9 @@
         <v>343</v>
       </c>
     </row>
-    <row r="168" spans="1:38">
+    <row r="168" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B168" t="s">
         <v>44</v>
@@ -15881,9 +15943,9 @@
         <v>344</v>
       </c>
     </row>
-    <row r="169" spans="1:38">
+    <row r="169" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B169" t="s">
         <v>45</v>
@@ -15997,9 +16059,9 @@
         <v>345</v>
       </c>
     </row>
-    <row r="170" spans="1:38">
+    <row r="170" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B170" t="s">
         <v>46</v>

</xml_diff>